<commit_message>
Cartelito mocho de alta cliente + verificar si ya toco el boton y trato de validar si existe en DB el el CBU
</commit_message>
<xml_diff>
--- a/TPINT_GRUPO_2_LAB4/lista de tareas labo4.xlsx
+++ b/TPINT_GRUPO_2_LAB4/lista de tareas labo4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guini\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guini\OneDrive\Documentos\Repositorios\TPFINAL-Grupo-2\TPINT_GRUPO_2_LAB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DD16884-9EDF-4AEC-A4FA-C529A0640A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C5C24F-F3FB-49D3-8AD7-EF6CE2931E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{322D9471-ED4E-41D4-9ACF-A24347DDBB13}"/>
   </bookViews>
@@ -201,12 +201,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,8 +227,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +558,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +580,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -584,7 +591,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">

</xml_diff>

<commit_message>
lista de tareas actualizada !IMPORTANTE! chequear
</commit_message>
<xml_diff>
--- a/TPINT_GRUPO_2_LAB4/lista de tareas labo4.xlsx
+++ b/TPINT_GRUPO_2_LAB4/lista de tareas labo4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guini\OneDrive\Documentos\Repositorios\TPFINAL-Grupo-2\TPINT_GRUPO_2_LAB4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dalam\OneDrive\Escritorio\Repositorio Eclipse\tpint_grupo_2\TPINT_GRUPO_2_LAB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C5C24F-F3FB-49D3-8AD7-EF6CE2931E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0332D753-7DB5-4F80-A56C-7E3A58F1F0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{322D9471-ED4E-41D4-9ACF-A24347DDBB13}"/>
+    <workbookView xWindow="5310" yWindow="420" windowWidth="23340" windowHeight="14745" xr2:uid="{322D9471-ED4E-41D4-9ACF-A24347DDBB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +200,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +219,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,14 +247,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -248,7 +288,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F2F4712-4441-47B5-9BD5-BDD5F85937DF}" name="Tabla1" displayName="Tabla1" ref="A1:B25" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F2F4712-4441-47B5-9BD5-BDD5F85937DF}" name="Tabla1" displayName="Tabla1" ref="A1:B25" totalsRowShown="0" tableBorderDxfId="0">
   <autoFilter ref="A1:B25" xr:uid="{6F2F4712-4441-47B5-9BD5-BDD5F85937DF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CADFA508-8E15-4246-9A3B-40B5B246422A}" name="nro"/>
@@ -558,29 +598,29 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="194.28515625" customWidth="1"/>
     <col min="4" max="4" width="199.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -588,10 +628,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -599,10 +639,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -610,10 +650,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
@@ -621,10 +661,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
@@ -632,10 +672,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
@@ -643,10 +683,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
@@ -654,10 +694,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
@@ -665,10 +705,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
@@ -676,10 +716,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
@@ -687,10 +727,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
@@ -698,10 +738,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
@@ -709,10 +749,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
@@ -720,10 +760,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="s">
@@ -731,10 +771,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
@@ -742,10 +782,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D17" t="s">
@@ -753,10 +793,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
@@ -764,10 +804,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D19" t="s">
@@ -775,10 +815,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
@@ -786,10 +826,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D21" t="s">
@@ -797,10 +837,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D22" t="s">
@@ -808,10 +848,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
@@ -819,10 +859,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
@@ -830,10 +870,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D25" t="s">
@@ -842,8 +882,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>